<commit_message>
Completed refreshing pivot tables with custom sorting.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableSorting.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableSorting.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8CF647F-F04B-43FA-A896-CE9521383347}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81997723-3D2D-4E1D-A3FA-A98FC7578570}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="9564" activeTab="3" xr2:uid="{B7885013-94A0-41CE-B230-E54384CEF231}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="9564" firstSheet="2" activeTab="4" xr2:uid="{B7885013-94A0-41CE-B230-E54384CEF231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="SortingWithoutReferences" sheetId="2" r:id="rId2"/>
     <sheet name="SortingWithReferencesRowFields" sheetId="3" r:id="rId3"/>
     <sheet name="RowColumnFieldsSorting" sheetId="4" r:id="rId4"/>
+    <sheet name="DataFieldsInRows" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="47">
   <si>
     <t>Transaction</t>
   </si>
@@ -155,6 +156,24 @@
   <si>
     <t>March Sum of Total</t>
   </si>
+  <si>
+    <t>Chicago Sum of Total</t>
+  </si>
+  <si>
+    <t>Nashville Sum of Total</t>
+  </si>
+  <si>
+    <t>San Francisco Sum of Total</t>
+  </si>
+  <si>
+    <t>January Total</t>
+  </si>
+  <si>
+    <t>February Total</t>
+  </si>
+  <si>
+    <t>March Total</t>
+  </si>
 </sst>
 </file>
 
@@ -229,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,6 +262,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -387,7 +409,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A0244332-D2BC-4283-8621-8F299A7CDE12}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A0244332-D2BC-4283-8621-8F299A7CDE12}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A16:W23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0" sortType="descending">
@@ -540,7 +562,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16A0DFA6-F08D-4B23-B34E-F2A7C173E669}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16A0DFA6-F08D-4B23-B34E-F2A7C173E669}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A18:S25" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -693,8 +715,601 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81B2F3CD-4990-41C0-8D6C-8EE15758BAA9}" name="PivotTable4" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A50:J84" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="8">
+        <item x="6"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="0"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="32">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E57A261-D0CB-4C51-BE2F-382229D2E8B6}" name="PivotTable3" cacheId="6" dataOnRows="1" dataPosition="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A33:J46" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="5">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2714B505-4162-4048-ADF2-10FA53A6BF5D}" name="PivotTable2" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A17:E29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E72314CB-1912-4BC2-9B98-7F7F6A0CE5D0}" name="PivotTable1" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE8F38F0-0A18-4D56-B5E6-AB059BC04FA1}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE8F38F0-0A18-4D56-B5E6-AB059BC04FA1}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -797,7 +1412,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E56F8794-8A21-42F4-9751-E363FE92B4F4}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E56F8794-8A21-42F4-9751-E363FE92B4F4}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A27:I40" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -922,189 +1537,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{745F5D76-15EB-488D-B996-85A7FD1932E0}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A23:C34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C855FFD-62F5-47E4-9FB1-F65E97F2E762}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A36B3B1-2793-447A-9C07-AB33BACEDA30}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A36B3B1-2793-447A-9C07-AB33BACEDA30}" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A38:C49" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1213,8 +1646,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB7573B6-E3C1-48C7-925F-04115E00B514}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB7573B6-E3C1-48C7-925F-04115E00B514}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A9:C19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1337,8 +1770,190 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{745F5D76-15EB-488D-B996-85A7FD1932E0}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A23:C34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C855FFD-62F5-47E4-9FB1-F65E97F2E762}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{170EA9EE-7729-4C9F-A62E-35FEF8426B6E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{170EA9EE-7729-4C9F-A62E-35FEF8426B6E}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A29:AH44" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -1585,7 +2200,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44B2FEDB-6162-4592-8D71-1E960C3523CB}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44B2FEDB-6162-4592-8D71-1E960C3523CB}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:K14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3514,7 +4129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867ADF89-83F9-4EA3-8474-EF3366DAFF9C}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -5065,4 +5680,1384 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD60FC-523D-4707-B2BA-74D0FBACA083}">
+  <dimension ref="A1:J84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6">
+        <v>99</v>
+      </c>
+      <c r="C5" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="E8" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1194</v>
+      </c>
+      <c r="C11" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1293</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="D13" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1194</v>
+      </c>
+      <c r="D20" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="E20" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="E23" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
+        <v>2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6">
+        <v>99</v>
+      </c>
+      <c r="D26" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="E26" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1293</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="E28" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="6">
+        <v>3</v>
+      </c>
+      <c r="C29" s="6">
+        <v>7</v>
+      </c>
+      <c r="D29" s="6">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6">
+        <v>99</v>
+      </c>
+      <c r="D37" s="6">
+        <v>99</v>
+      </c>
+      <c r="E37" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="F37" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1194</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6">
+        <v>1194</v>
+      </c>
+      <c r="E40" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F40" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I40" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="J40" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="6">
+        <v>6</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6">
+        <v>6</v>
+      </c>
+      <c r="E41" s="6">
+        <v>2</v>
+      </c>
+      <c r="F41" s="6">
+        <v>2</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6">
+        <v>2</v>
+      </c>
+      <c r="I41" s="6">
+        <v>2</v>
+      </c>
+      <c r="J41" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F43" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G43" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="J43" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6">
+        <v>2</v>
+      </c>
+      <c r="F44" s="6">
+        <v>2</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6">
+        <v>1</v>
+      </c>
+      <c r="J44" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1194</v>
+      </c>
+      <c r="C45" s="6">
+        <v>99</v>
+      </c>
+      <c r="D45" s="6">
+        <v>1293</v>
+      </c>
+      <c r="E45" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="F45" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="G45" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H45" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I45" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="J45" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="6">
+        <v>6</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6">
+        <v>7</v>
+      </c>
+      <c r="E46" s="6">
+        <v>5</v>
+      </c>
+      <c r="F46" s="6">
+        <v>5</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+      <c r="H46" s="6">
+        <v>2</v>
+      </c>
+      <c r="I46" s="6">
+        <v>3</v>
+      </c>
+      <c r="J46" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>20100090</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F55" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6">
+        <v>2</v>
+      </c>
+      <c r="F56" s="6">
+        <v>2</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>20100070</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6">
+        <v>1194</v>
+      </c>
+      <c r="D58" s="6">
+        <v>1194</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6">
+        <v>6</v>
+      </c>
+      <c r="D59" s="6">
+        <v>6</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>20100017</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I61" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="J61" s="6">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6">
+        <v>2</v>
+      </c>
+      <c r="I62" s="6">
+        <v>2</v>
+      </c>
+      <c r="J62" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6">
+        <v>1194</v>
+      </c>
+      <c r="D63" s="6">
+        <v>1194</v>
+      </c>
+      <c r="E63" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F63" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I63" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="J63" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6">
+        <v>6</v>
+      </c>
+      <c r="D64" s="6">
+        <v>6</v>
+      </c>
+      <c r="E64" s="6">
+        <v>2</v>
+      </c>
+      <c r="F64" s="6">
+        <v>2</v>
+      </c>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6">
+        <v>2</v>
+      </c>
+      <c r="I64" s="6">
+        <v>2</v>
+      </c>
+      <c r="J64" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
+        <v>20100083</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="J67" s="6">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6">
+        <v>1</v>
+      </c>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6">
+        <v>1</v>
+      </c>
+      <c r="J68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>20100007</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F70" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6">
+        <v>2</v>
+      </c>
+      <c r="F71" s="6">
+        <v>2</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F72" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G72" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="J72" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6">
+        <v>2</v>
+      </c>
+      <c r="F73" s="6">
+        <v>2</v>
+      </c>
+      <c r="G73" s="6">
+        <v>1</v>
+      </c>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6">
+        <v>1</v>
+      </c>
+      <c r="J73" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>20100085</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="6">
+        <v>99</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6">
+        <v>99</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6">
+        <v>1</v>
+      </c>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
+        <v>20100076</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="F79" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6">
+        <v>1</v>
+      </c>
+      <c r="F80" s="6">
+        <v>1</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="6">
+        <v>99</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6">
+        <v>99</v>
+      </c>
+      <c r="E81" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="F81" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" s="6">
+        <v>1</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6">
+        <v>1</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6">
+        <v>1</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" s="6">
+        <v>99</v>
+      </c>
+      <c r="C83" s="6">
+        <v>1194</v>
+      </c>
+      <c r="D83" s="6">
+        <v>1293</v>
+      </c>
+      <c r="E83" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="F83" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="G83" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H83" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I83" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="J83" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="6">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6">
+        <v>6</v>
+      </c>
+      <c r="D84" s="6">
+        <v>7</v>
+      </c>
+      <c r="E84" s="6">
+        <v>5</v>
+      </c>
+      <c r="F84" s="6">
+        <v>5</v>
+      </c>
+      <c r="G84" s="6">
+        <v>1</v>
+      </c>
+      <c r="H84" s="6">
+        <v>2</v>
+      </c>
+      <c r="I84" s="6">
+        <v>3</v>
+      </c>
+      <c r="J84" s="6">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>